<commit_message>
Add description to retrieve.py
</commit_message>
<xml_diff>
--- a/src/resources/agents.xlsx
+++ b/src/resources/agents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\python\covidProject\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B8EA75-F9E0-4BF2-80C1-855B94B5A330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F09483B-6ECD-456A-8941-8477510517C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="600" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7760" uniqueCount="3779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7764" uniqueCount="3781">
   <si>
     <t>handle</t>
   </si>
@@ -11358,6 +11358,12 @@
   </si>
   <si>
     <t>error_code</t>
+  </si>
+  <si>
+    <t>user does not exist</t>
+  </si>
+  <si>
+    <t>user suspended</t>
   </si>
 </sst>
 </file>
@@ -11409,11 +11415,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11720,8 +11727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2404" workbookViewId="0">
-      <selection activeCell="I2414" sqref="I2414"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -45964,15 +45971,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C03D278-41EB-4F7B-9244-BA716EC6CBB5}">
-  <dimension ref="A1:D106"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -45986,7 +45993,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3671</v>
       </c>
@@ -45999,8 +46006,14 @@
       <c r="D2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>3672</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3779</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3673</v>
       </c>
@@ -46013,8 +46026,14 @@
       <c r="D3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>3676</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>3780</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3674</v>
       </c>
@@ -46028,7 +46047,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3675</v>
       </c>
@@ -46042,7 +46061,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3677</v>
       </c>
@@ -46056,7 +46075,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3678</v>
       </c>
@@ -46070,7 +46089,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3679</v>
       </c>
@@ -46084,7 +46103,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3680</v>
       </c>
@@ -46098,7 +46117,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>3681</v>
       </c>
@@ -46112,7 +46131,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>3682</v>
       </c>
@@ -46126,7 +46145,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>3683</v>
       </c>
@@ -46140,7 +46159,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3684</v>
       </c>
@@ -46154,7 +46173,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>3685</v>
       </c>
@@ -46168,7 +46187,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>3686</v>
       </c>
@@ -46182,7 +46201,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>3687</v>
       </c>
@@ -47458,5 +47477,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>